<commit_message>
Actualizando API con Funciones de la Bd e insertando script con creación de funciones
</commit_message>
<xml_diff>
--- a/InfoProyecto/DataExcel/Indicadores APP Mobile.xlsx
+++ b/InfoProyecto/DataExcel/Indicadores APP Mobile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Trabajo\InfoProyecto\DataExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A92CC0-E37C-4CD7-B7EC-51935E7CEFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25373B7E-1B0A-4981-9556-2AECC93EE02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5C61D0CB-9E5D-4414-A367-E01C83CFC4AD}"/>
+    <workbookView xWindow="5868" yWindow="-48" windowWidth="17280" windowHeight="8964" xr2:uid="{5C61D0CB-9E5D-4414-A367-E01C83CFC4AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
-  <si>
-    <t>Capacidad de albergue</t>
-  </si>
-  <si>
-    <t>Capacidad instalada</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
   <si>
     <t>Edad</t>
   </si>
@@ -139,9 +133,6 @@
     <t>TIPO</t>
   </si>
   <si>
-    <t>CAMPO</t>
-  </si>
-  <si>
     <t>TOTAL</t>
   </si>
   <si>
@@ -173,6 +164,12 @@
   </si>
   <si>
     <t xml:space="preserve"> Población según edad simple(total)</t>
+  </si>
+  <si>
+    <t>VARIABLES</t>
+  </si>
+  <si>
+    <t>estado civil</t>
   </si>
 </sst>
 </file>
@@ -436,38 +433,38 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -806,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B3740D-FAA0-4173-A604-8099B0135A4E}">
   <dimension ref="B2:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="89" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
@@ -819,314 +816,312 @@
     <col min="6" max="6" width="53.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="31.5">
-      <c r="B2" s="15" t="s">
+    <row r="2" spans="2:5" ht="30">
+      <c r="B2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18"/>
+    </row>
+    <row r="3" spans="2:5" ht="22.8">
+      <c r="B3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="15.9" customHeight="1">
+      <c r="B4" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="15.9" customHeight="1">
+      <c r="B5" s="21"/>
+      <c r="C5" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="2:5" ht="15.9" customHeight="1">
+      <c r="B6" s="21"/>
+      <c r="C6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="2:5" ht="15.9" customHeight="1">
+      <c r="B7" s="21"/>
+      <c r="C7" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="19"/>
+    </row>
+    <row r="8" spans="2:5" ht="15.9" customHeight="1">
+      <c r="B8" s="21"/>
+      <c r="C8" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="19"/>
+    </row>
+    <row r="9" spans="2:5" ht="15.9" customHeight="1">
+      <c r="B9" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="15.9" customHeight="1">
+      <c r="B10" s="22"/>
+      <c r="C10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="20"/>
+    </row>
+    <row r="11" spans="2:5" ht="15.9" customHeight="1">
+      <c r="B11" s="22"/>
+      <c r="C11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="20"/>
+    </row>
+    <row r="12" spans="2:5" ht="15.9" customHeight="1">
+      <c r="B12" s="22"/>
+      <c r="C12" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="20"/>
+    </row>
+    <row r="13" spans="2:5" ht="15.9" customHeight="1">
+      <c r="B13" s="22"/>
+      <c r="C13" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="20"/>
+    </row>
+    <row r="14" spans="2:5" ht="15.9" customHeight="1">
+      <c r="B14" s="22"/>
+      <c r="C14" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="20"/>
+    </row>
+    <row r="15" spans="2:5" ht="15.9" customHeight="1">
+      <c r="B15" s="22"/>
+      <c r="C15" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="20"/>
+    </row>
+    <row r="16" spans="2:5" ht="15.9" customHeight="1">
+      <c r="B16" s="22"/>
+      <c r="C16" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="20"/>
+    </row>
+    <row r="17" spans="2:5" ht="15.9" customHeight="1">
+      <c r="B17" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="15.9" customHeight="1">
+      <c r="B18" s="21"/>
+      <c r="C18" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="19"/>
+    </row>
+    <row r="19" spans="2:5" ht="15.9" customHeight="1">
+      <c r="B19" s="21"/>
+      <c r="C19" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17"/>
-    </row>
-    <row r="3" spans="2:5" ht="24">
-      <c r="B3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="D19" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="19"/>
+    </row>
+    <row r="20" spans="2:5" ht="15.9" customHeight="1">
+      <c r="B20" s="21"/>
+      <c r="C20" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="19"/>
+    </row>
+    <row r="21" spans="2:5" ht="15.9" customHeight="1">
+      <c r="B21" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B4" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="12">
+      <c r="E21" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="15.9" customHeight="1">
+      <c r="B22" s="22"/>
+      <c r="C22" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="20"/>
+    </row>
+    <row r="23" spans="2:5" ht="15.9" customHeight="1">
+      <c r="B23" s="22"/>
+      <c r="C23" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="20"/>
+    </row>
+    <row r="24" spans="2:5" ht="15.9" customHeight="1">
+      <c r="B24" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="19">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B5" s="13"/>
-      <c r="C5" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B6" s="13"/>
-      <c r="C6" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="8" t="s">
+    <row r="25" spans="2:5" ht="15.9" customHeight="1">
+      <c r="B25" s="21"/>
+      <c r="C25" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="19"/>
+    </row>
+    <row r="26" spans="2:5" ht="15.9" customHeight="1">
+      <c r="B26" s="21"/>
+      <c r="C26" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="19"/>
+    </row>
+    <row r="27" spans="2:5" ht="15.9" customHeight="1">
+      <c r="B27" s="21"/>
+      <c r="C27" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="12"/>
-    </row>
-    <row r="7" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B7" s="13"/>
-      <c r="C7" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B8" s="13"/>
-      <c r="C8" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="12"/>
-    </row>
-    <row r="9" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B9" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="18">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B10" s="14"/>
-      <c r="C10" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="18"/>
-    </row>
-    <row r="11" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B11" s="14"/>
-      <c r="C11" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="18"/>
-    </row>
-    <row r="12" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B12" s="14"/>
-      <c r="C12" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="18"/>
-    </row>
-    <row r="13" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B13" s="14"/>
-      <c r="C13" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="18"/>
-    </row>
-    <row r="14" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B14" s="14"/>
-      <c r="C14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="18"/>
-    </row>
-    <row r="15" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B15" s="14"/>
-      <c r="C15" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="18"/>
-    </row>
-    <row r="16" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B16" s="14"/>
-      <c r="C16" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="18"/>
-    </row>
-    <row r="17" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B17" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" s="12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B18" s="13"/>
-      <c r="C18" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="12"/>
-    </row>
-    <row r="19" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B19" s="13"/>
-      <c r="C19" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="12"/>
-    </row>
-    <row r="20" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B20" s="13"/>
-      <c r="C20" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="12"/>
-    </row>
-    <row r="21" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B21" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B22" s="14"/>
-      <c r="C22" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="18"/>
-    </row>
-    <row r="23" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B23" s="14"/>
-      <c r="C23" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="18"/>
-    </row>
-    <row r="24" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B24" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E24" s="12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B25" s="13"/>
-      <c r="C25" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" s="12"/>
-    </row>
-    <row r="26" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B26" s="13"/>
-      <c r="C26" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E26" s="12"/>
-    </row>
-    <row r="27" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B27" s="13"/>
-      <c r="C27" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="12"/>
+      <c r="E27" s="19"/>
     </row>
     <row r="28" spans="2:5" ht="15.75" customHeight="1">
       <c r="B28" s="2"/>
     </row>
     <row r="30" spans="2:5" ht="14.4">
       <c r="B30" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="2:5" ht="14.4">
       <c r="B31" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="E4:E8"/>
-    <mergeCell ref="E9:E16"/>
-    <mergeCell ref="E17:E20"/>
-    <mergeCell ref="E21:E23"/>
     <mergeCell ref="E24:E27"/>
     <mergeCell ref="B24:B27"/>
     <mergeCell ref="B4:B8"/>
     <mergeCell ref="B17:B20"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="B9:B16"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="E4:E8"/>
+    <mergeCell ref="E9:E16"/>
+    <mergeCell ref="E17:E20"/>
+    <mergeCell ref="E21:E23"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="70" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Subiendo cambios finales del prototipo
</commit_message>
<xml_diff>
--- a/InfoProyecto/DataExcel/Indicadores APP Mobile.xlsx
+++ b/InfoProyecto/DataExcel/Indicadores APP Mobile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Trabajo\InfoProyecto\DataExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25373B7E-1B0A-4981-9556-2AECC93EE02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F46F32D-FA7B-44CA-8115-27A0CA1137D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5868" yWindow="-48" windowWidth="17280" windowHeight="8964" xr2:uid="{5C61D0CB-9E5D-4414-A367-E01C83CFC4AD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5C61D0CB-9E5D-4414-A367-E01C83CFC4AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -445,6 +445,15 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -454,16 +463,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -804,7 +804,7 @@
   <dimension ref="B2:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="89" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
@@ -817,12 +817,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="30">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
     </row>
     <row r="3" spans="2:5" ht="22.8">
       <c r="B3" s="3" t="s">
@@ -839,59 +839,59 @@
       </c>
     </row>
     <row r="4" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="17" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="16">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B5" s="21"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="19"/>
+      <c r="E5" s="16"/>
     </row>
     <row r="6" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B6" s="21"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="19"/>
+      <c r="E6" s="16"/>
     </row>
     <row r="7" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B7" s="21"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="10" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="19"/>
+      <c r="E7" s="16"/>
     </row>
     <row r="8" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B8" s="21"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="12" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="19"/>
+      <c r="E8" s="16"/>
     </row>
     <row r="9" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="18" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -900,82 +900,82 @@
       <c r="D9" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="22">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B10" s="22"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="20"/>
+      <c r="E10" s="22"/>
     </row>
     <row r="11" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B11" s="22"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="20"/>
+      <c r="E11" s="22"/>
     </row>
     <row r="12" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B12" s="22"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="11" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="20"/>
+      <c r="E12" s="22"/>
     </row>
     <row r="13" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B13" s="22"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="11" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="20"/>
+      <c r="E13" s="22"/>
     </row>
     <row r="14" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B14" s="22"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="11" t="s">
         <v>20</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="20"/>
+      <c r="E14" s="22"/>
     </row>
     <row r="15" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B15" s="22"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="11" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="20"/>
+      <c r="E15" s="22"/>
     </row>
     <row r="16" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B16" s="22"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="12" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="20"/>
+      <c r="E16" s="22"/>
     </row>
     <row r="17" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="17" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="11" t="s">
@@ -984,42 +984,42 @@
       <c r="D17" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E17" s="16">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B18" s="21"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="19"/>
+      <c r="E18" s="16"/>
     </row>
     <row r="19" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B19" s="21"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="19"/>
+      <c r="E19" s="16"/>
     </row>
     <row r="20" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B20" s="21"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="19"/>
+      <c r="E20" s="16"/>
     </row>
     <row r="21" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="18" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -1028,32 +1028,32 @@
       <c r="D21" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="20">
+      <c r="E21" s="22">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B22" s="22"/>
+      <c r="B22" s="18"/>
       <c r="C22" s="10" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E22" s="20"/>
+      <c r="E22" s="22"/>
     </row>
     <row r="23" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B23" s="22"/>
+      <c r="B23" s="18"/>
       <c r="C23" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="20"/>
+      <c r="E23" s="22"/>
     </row>
     <row r="24" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="17" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="10" t="s">
@@ -1062,39 +1062,39 @@
       <c r="D24" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="19">
+      <c r="E24" s="16">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B25" s="21"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="19"/>
+      <c r="E25" s="16"/>
     </row>
     <row r="26" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B26" s="21"/>
+      <c r="B26" s="17"/>
       <c r="C26" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="19"/>
+      <c r="E26" s="16"/>
     </row>
     <row r="27" spans="2:5" ht="15.9" customHeight="1">
-      <c r="B27" s="21"/>
+      <c r="B27" s="17"/>
       <c r="C27" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E27" s="19"/>
+      <c r="E27" s="16"/>
     </row>
     <row r="28" spans="2:5" ht="15.75" customHeight="1">
       <c r="B28" s="2"/>
@@ -1111,17 +1111,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="E4:E8"/>
+    <mergeCell ref="E9:E16"/>
+    <mergeCell ref="E17:E20"/>
+    <mergeCell ref="E21:E23"/>
     <mergeCell ref="E24:E27"/>
     <mergeCell ref="B24:B27"/>
     <mergeCell ref="B4:B8"/>
     <mergeCell ref="B17:B20"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="B9:B16"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="E4:E8"/>
-    <mergeCell ref="E9:E16"/>
-    <mergeCell ref="E17:E20"/>
-    <mergeCell ref="E21:E23"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="70" orientation="landscape" r:id="rId1"/>

</xml_diff>